<commit_message>
Removed useless language profiles
</commit_message>
<xml_diff>
--- a/docs/LanguageSupport.xlsx
+++ b/docs/LanguageSupport.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mIHA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Java\LATINO4J\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
   <si>
     <t>EN</t>
   </si>
@@ -83,15 +83,6 @@
     <t>EL</t>
   </si>
   <si>
-    <t>LT</t>
-  </si>
-  <si>
-    <t>LV</t>
-  </si>
-  <si>
-    <t>MT</t>
-  </si>
-  <si>
     <t>PL</t>
   </si>
   <si>
@@ -177,15 +168,6 @@
   </si>
   <si>
     <t>Greek</t>
-  </si>
-  <si>
-    <t>Lithuanian</t>
-  </si>
-  <si>
-    <t>Latvian</t>
-  </si>
-  <si>
-    <t>Maltese</t>
   </si>
   <si>
     <t>Polish</t>
@@ -564,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,22 +563,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -604,22 +586,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -627,22 +609,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -650,19 +632,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -670,19 +652,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -690,19 +672,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -710,19 +692,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -730,19 +712,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -750,19 +732,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -770,19 +752,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -790,19 +772,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -810,19 +792,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -830,19 +812,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -850,22 +829,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -873,22 +849,22 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -896,16 +872,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -913,19 +886,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -933,19 +903,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -953,22 +923,22 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -976,10 +946,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -987,10 +957,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -998,10 +974,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1009,10 +991,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1020,16 +1005,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1037,16 +1016,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1054,13 +1030,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" t="s">
-        <v>61</v>
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1068,10 +1044,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1079,87 +1061,39 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
         <v>58</v>
       </c>
-      <c r="D29" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" t="s">
-        <v>61</v>
+      <c r="F29" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" t="s">
         <v>61</v>
       </c>
-      <c r="E30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" t="s">
-        <v>61</v>
+      <c r="F30" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B34" s="1"/>
+      <c r="B31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EE is actually Estonian (now renamed to ET)
</commit_message>
<xml_diff>
--- a/docs/LanguageSupport.xlsx
+++ b/docs/LanguageSupport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="63">
   <si>
     <t>EN</t>
   </si>
@@ -195,12 +195,6 @@
   </si>
   <si>
     <t>Portuguese</t>
-  </si>
-  <si>
-    <t>EE</t>
-  </si>
-  <si>
-    <t>Ewe (Niger-Congo)</t>
   </si>
   <si>
     <t>Slovak</t>
@@ -546,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,13 +566,13 @@
         <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -880,6 +874,9 @@
       <c r="E16" t="s">
         <v>55</v>
       </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -974,7 +971,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
         <v>55</v>
@@ -1072,28 +1069,17 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F29" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="1"/>
+      <c r="B30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>